<commit_message>
Add progress bars, add event 'available free translations', fix sizes of windows
</commit_message>
<xml_diff>
--- a/book_zh_en_ru.xlsx
+++ b/book_zh_en_ru.xlsx
@@ -1740,257 +1740,257 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Yang Zhi Manlu Price Increase Permission</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Old Times</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Strawberry Muffin Price Increase License</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Self-serve</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>sunglasses</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Potato Bun Price Increase License</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>A letter with graffiti.</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Wishing Gems</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Permission to increase the price of porridge rice</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Shiba Dog Hat</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>video game</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Idol 101 Letter</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Curry Rice Price Increase License</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Banknote</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Price increase permit for red bean gardenia</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Mushroom Pasta Price Increase License</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Butter Bread Price Increase License</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Pig's nose.</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Price Increase License for Spicy Rice and Milk</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Price Increase License for Steamed Clams</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Scarves and Badges</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Letter from Auntie's son.</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Notebook</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>A catch clip</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>fantasy refrigerator</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>pocket watch</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>fantasy liquor cabinet</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>sausage mouth</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>greedy cylinder</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>rainbow sticker</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Greedy cat</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Coffee</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Uniform Yorkshire Baby Doll</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Fantasy Coffee Table</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Picnic Hanging Ears Rabbit Doll</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>fantasy fence</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Hip-Hop Toad Doll</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>White Peach Oolong Tea</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Fantasy Dining Table</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Kimono Goose Doll</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Tuna sushi</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Sweet love.</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Auntie Girl Doll</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>floating tea cup</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Hide Monuments</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Penguin Painter Doll</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Sports Dog Doll</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -2532,262 +2532,262 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Грибная страсть</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 30 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Ян Чжи Маньлу Разрешение на повышение цены</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Старые добрые времена</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Лицензия на увеличение цены на клубничный кекс</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Самообслуживание</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>солнцезащитные очки</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Лицензия на повышение цены на картофельную булочку</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Письмо с граффити.</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Желающие драгоценные камни</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Разрешение на повышение цены риса каши</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Шляпа для собак Shiba</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>видеоигра</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Буква идола 101</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Лицензия на увеличение цены на рис с карри</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Банкнота</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Разрешение на повышение цен на красную фасоль GARDIIA</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Лицензия на увеличение цены на грибную пасту</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Лицензия на повышение цены на хлеб</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Свиной нос.</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Лицензия на увеличение цен на пряный рис и молоко</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Лицензия на увеличение цены на паровые моллюски</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Шарфы и значки</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Письмо от сына тети.</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Ноутбук</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Фиксирующий зажим</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>фэнтези холодильник</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Карманные часы</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>шкаф для выпивки фэнтези</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>сосисочный рот</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>жадный цилиндр</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>радужная наклейка</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Жадная кошка</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Кофе</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Детская кукла Yorkshire Uniform</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Журнальный столик Fantasy</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Кукла с кроличьими ушками для пикника</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>fantasy fence</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Кукла хип-хоп жаба</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Белый персиковый улун</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Обеденный стол Fantasy</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Кимоно-гусиная кукла</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Суши тунец</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Милая любовь.</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Кукла для тётушек</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>чашка для чая</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Скрыть памятники</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Кукла Penguin Painter</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Спортивная кукла для собак</t>
+          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>

</xml_diff>

<commit_message>
fix IF in stop condition
</commit_message>
<xml_diff>
--- a/book_zh_en_ru.xlsx
+++ b/book_zh_en_ru.xlsx
@@ -1740,257 +1740,257 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Yang Zhi Manlu Price Increase Permission</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Old Times</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Strawberry Muffin Price Increase License</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Self-serve</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>sunglasses</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Potato Bun Price Increase License</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>A letter with graffiti.</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Wishing Gems</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Permission to increase the price of porridge rice</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Shiba Dog Hat</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>video game</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Idol 101 Letter</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Curry Rice Price Increase License</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Banknote</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Price increase permit for red bean gardenia</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Mushroom Pasta Price Increase License</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Butter Bread Price Increase License</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Pig's nose.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Price Increase License for Spicy Rice and Milk</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Price Increase License for Steamed Clams</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Scarves and Badges</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Letter from Auntie's son.</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Notebook</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>A catch clip</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>fantasy refrigerator</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>pocket watch</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>fantasy liquor cabinet</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>sausage mouth</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>greedy cylinder</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>rainbow sticker</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Greedy cat</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Coffee</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Uniform Yorkshire Baby Doll</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Fantasy Coffee Table</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Picnic Hanging Ears Rabbit Doll</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>fantasy fence</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Hip-Hop Toad Doll</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>White Peach Oolong Tea</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Fantasy Dining Table</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Kimono Goose Doll</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Tuna sushi</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Sweet love.</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Auntie Girl Doll</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>floating tea cup</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Hide Monuments</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Penguin Painter Doll</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Sports Dog Doll</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -2532,262 +2532,262 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 30 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Грибная страсть</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Ян Чжи Маньлу Разрешение на повышение цены</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Старые добрые времена</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Лицензия на увеличение цены на клубничный кекс</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Самообслуживание</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 29 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>солнцезащитные очки</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Лицензия на повышение цены на картофельную булочку</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Письмо с граффити.</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Желающие драгоценные камни</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Разрешение на повышение цены риса каши</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 28 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Шляпа для собак Shiba</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>видеоигра</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Буква идола 101</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Лицензия на увеличение цены на рис с карри</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Банкнота</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Разрешение на повышение цен на красную фасоль GARDIIA</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 27 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Лицензия на увеличение цены на грибную пасту</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Лицензия на повышение цены на хлеб</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Свиной нос.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Лицензия на увеличение цен на пряный рис и молоко</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Лицензия на увеличение цены на паровые моллюски</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 26 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Шарфы и значки</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Письмо от сына тети.</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Ноутбук</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Фиксирующий зажим</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>фэнтези холодильник</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Карманные часы</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 25 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>шкаф для выпивки фэнтези</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>сосисочный рот</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>жадный цилиндр</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>радужная наклейка</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Жадная кошка</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 24 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Кофе</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Детская кукла Yorkshire Uniform</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Журнальный столик Fantasy</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Кукла с кроличьими ушками для пикника</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>fantasy fence</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 23 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Кукла хип-хоп жаба</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Белый персиковый улун</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Обеденный стол Fantasy</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Кимоно-гусиная кукла</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Суши тунец</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 22 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Милая любовь.</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Кукла для тётушек</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>чашка для чая</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Скрыть памятники</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Кукла Penguin Painter</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>MYMEMORY WARNING: YOU USED ALL AVAILABLE FREE TRANSLATIONS FOR TODAY. NEXT AVAILABLE IN  16 HOURS 37 MINUTES 21 SECONDS VISIT HTTPS://MYMEMORY.TRANSLATED.NET/DOC/USAGELIMITS.PHP TO TRANSLATE MORE</t>
+          <t>Спортивная кукла для собак</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>

</xml_diff>